<commit_message>
Initial commit - upload project
</commit_message>
<xml_diff>
--- a/TC17_ApprovedRequest/17_ActionAlertMessage_ApprovedRequest.xlsx
+++ b/TC17_ApprovedRequest/17_ActionAlertMessage_ApprovedRequest.xlsx
@@ -1,21 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\test2\it\Project_Test_AcademicService\TC17_ApprovedRequest\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA83E1BA-88D9-406B-A79B-CA7756D97538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="0"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TC17-EC" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="TC17-TC" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TC17-EC" sheetId="1" r:id="rId1"/>
+    <sheet name="TC17-TC" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>TCID</t>
   </si>
@@ -186,99 +205,101 @@
   </si>
   <si>
     <t>อนุมัติ</t>
+  </si>
+  <si>
+    <t>Valid Da ApprovedRequest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="9">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
       <charset val="222"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <b val="1"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Tahoma"/>
+      <family val="2"/>
       <charset val="222"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Tahoma"/>
+      <family val="2"/>
       <charset val="222"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="TH Sarabun ps"/>
       <charset val="222"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Tahoma"/>
+      <family val="2"/>
       <charset val="222"/>
-      <family val="2"/>
-      <color rgb="FF00B050"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.1499984740745262"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.09997863704336681"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,7 +316,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.5999938962981048"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,138 +460,138 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
     <cellStyle name="เปอร์เซ็นต์" xfId="1" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.5999633777886288"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -583,7 +604,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
       </font>
       <fill>
         <patternFill>
@@ -593,10 +614,18 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="1">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="1" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -916,28 +945,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C1" sqref="C1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col width="9.83203125" customWidth="1" style="42" min="1" max="1"/>
-    <col width="27.9140625" customWidth="1" style="42" min="2" max="2"/>
-    <col width="27.25" customWidth="1" style="42" min="3" max="3"/>
-    <col width="20.6640625" customWidth="1" style="42" min="4" max="4"/>
-    <col width="9.33203125" customWidth="1" style="42" min="5" max="5"/>
-    <col width="30.75" customWidth="1" style="42" min="6" max="6"/>
-    <col width="28.08203125" customWidth="1" style="42" min="7" max="7"/>
-    <col width="21.83203125" customWidth="1" style="42" min="8" max="8"/>
-    <col width="27.75" customWidth="1" style="42" min="9" max="9"/>
+    <col min="1" max="1" width="9.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.9140625" customWidth="1"/>
+    <col min="3" max="3" width="27.25" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="30.75" customWidth="1"/>
+    <col min="7" max="7" width="28.08203125" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="27.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -969,8 +994,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="52.5" customHeight="1" s="42">
-      <c r="A2" s="5" t="n">
+    <row r="2" spans="1:9" ht="52.5" customHeight="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -982,7 +1007,7 @@
       <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="5" t="n">
+      <c r="E2" s="5">
         <v>1</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -998,8 +1023,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="58" customHeight="1" s="42">
-      <c r="A3" s="5" t="n">
+    <row r="3" spans="1:9" ht="58" customHeight="1">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1011,7 +1036,7 @@
       <c r="D3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="5" t="n">
+      <c r="E3" s="5">
         <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -1031,7 +1056,8 @@
       <c r="E6" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="F6" s="42"/>
+      <c r="G6" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1041,11 +1067,11 @@
       </c>
       <c r="F7" s="6">
         <f>COUNTIF(G2:G3, "Pass")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G7" s="12">
         <f>F7*100/F9</f>
-        <v/>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -1054,11 +1080,11 @@
       </c>
       <c r="F8" s="6">
         <f>COUNTIF(G2:G3, "FAIL")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G8" s="13">
         <f>F8*100/F9</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1067,27 +1093,28 @@
       </c>
       <c r="F9" s="14">
         <f>SUM(F7+F8)</f>
-        <v/>
-      </c>
-      <c r="G9" s="15" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="15">
         <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="E10" s="9" t="n"/>
-      <c r="F10" s="9" t="n"/>
-      <c r="G10" s="9" t="n"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="E11" s="9" t="n"/>
-      <c r="F11" s="9" t="n"/>
-      <c r="G11" s="9" t="n"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:9">
       <c r="E12" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="41" t="s">
+      <c r="F12" s="42"/>
+      <c r="G12" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1097,11 +1124,11 @@
       </c>
       <c r="F13" s="6">
         <f>COUNTIF(H2:H3, "PASS")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="G13" s="12">
         <f>F13*100/F15</f>
-        <v/>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1110,11 +1137,11 @@
       </c>
       <c r="F14" s="6">
         <f>COUNTIF(H2:H3, "FAIL")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G14" s="13">
         <f>F14*100/F15</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1123,9 +1150,9 @@
       </c>
       <c r="F15" s="14">
         <f>SUM(F13+F14)</f>
-        <v/>
-      </c>
-      <c r="G15" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="G15" s="12">
         <v>100</v>
       </c>
     </row>
@@ -1135,10 +1162,10 @@
     <mergeCell ref="E12:F12"/>
   </mergeCells>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="1">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="2" operator="equal" dxfId="0">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1147,25 +1174,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col width="12.1640625" customWidth="1" style="42" min="1" max="1"/>
-    <col width="26.08203125" customWidth="1" style="42" min="2" max="2"/>
-    <col width="34.6640625" customWidth="1" style="42" min="3" max="3"/>
-    <col width="31.08203125" customWidth="1" style="42" min="4" max="4"/>
-    <col width="24.25" customWidth="1" style="42" min="5" max="5"/>
-    <col width="27.58203125" customWidth="1" style="42" min="6" max="6"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.08203125" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.08203125" customWidth="1"/>
+    <col min="5" max="5" width="24.25" customWidth="1"/>
+    <col min="6" max="6" width="27.58203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1188,12 +1211,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16.5" customHeight="1" s="42">
-      <c r="A2" s="16" t="n">
+    <row r="2" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>30</v>
@@ -1201,23 +1224,26 @@
       <c r="D2" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="34" t="n"/>
+      <c r="E2" s="34"/>
       <c r="F2" s="43" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="33.5" customHeight="1" s="42">
-      <c r="A3" s="45" t="n"/>
+    <row r="3" spans="1:6" ht="33.5" customHeight="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="35" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="36" t="n"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="B4" s="23" t="n"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="24" t="s">
         <v>34</v>
       </c>
@@ -1227,9 +1253,11 @@
       <c r="E4" s="37" t="s">
         <v>36</v>
       </c>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="B5" s="23" t="n"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="24" t="s">
         <v>37</v>
       </c>
@@ -1239,39 +1267,47 @@
       <c r="E5" s="38" t="s">
         <v>39</v>
       </c>
+      <c r="F5" s="42"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="B6" s="23" t="n"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="32" t="n"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="42"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="B7" s="23" t="n"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="21" t="s">
         <v>42</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="32" t="n"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="42"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="B8" s="25" t="n"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="32" t="n"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="42"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="B9" s="25" t="n"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="22" t="s">
         <v>46</v>
       </c>
@@ -1281,9 +1317,11 @@
       <c r="E9" s="32" t="s">
         <v>9</v>
       </c>
+      <c r="F9" s="42"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="B10" s="25" t="n"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="22" t="s">
         <v>48</v>
       </c>
@@ -1293,18 +1331,21 @@
       <c r="E10" s="40" t="s">
         <v>50</v>
       </c>
+      <c r="F10" s="42"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="B11" s="29" t="n"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="28" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="33" t="n"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.5" customHeight="1" s="42">
+      <c r="E11" s="33"/>
+      <c r="F11" s="42"/>
+    </row>
+    <row r="12" spans="1:6" ht="16.5" customHeight="1">
       <c r="A12" s="16" t="s">
         <v>53</v>
       </c>
@@ -1317,24 +1358,26 @@
       <c r="D12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="34" t="n"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" s="42">
-      <c r="A13" s="19" t="n"/>
+    <row r="13" spans="1:6" ht="16.5" customHeight="1">
+      <c r="A13" s="19"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="35" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="36" t="n"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="42"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="22" t="n"/>
-      <c r="B14" s="23" t="n"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="24" t="s">
         <v>34</v>
       </c>
@@ -1344,10 +1387,11 @@
       <c r="E14" s="37" t="s">
         <v>36</v>
       </c>
+      <c r="F14" s="42"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="22" t="n"/>
-      <c r="B15" s="23" t="n"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="24" t="s">
         <v>37</v>
       </c>
@@ -1357,42 +1401,46 @@
       <c r="E15" s="38" t="s">
         <v>39</v>
       </c>
+      <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="22" t="n"/>
-      <c r="B16" s="23" t="n"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="22" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="32" t="n"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="22" t="n"/>
-      <c r="B17" s="23" t="n"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="21" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="32" t="n"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="22" t="n"/>
-      <c r="B18" s="25" t="n"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="28" customHeight="1" s="42">
-      <c r="A19" s="22" t="n"/>
-      <c r="B19" s="25" t="n"/>
+      <c r="F18" s="42"/>
+    </row>
+    <row r="19" spans="1:6" ht="28" customHeight="1">
+      <c r="A19" s="22"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="22" t="s">
         <v>46</v>
       </c>
@@ -1402,10 +1450,11 @@
       <c r="E19" s="39" t="s">
         <v>15</v>
       </c>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="22" t="n"/>
-      <c r="B20" s="25" t="n"/>
+      <c r="A20" s="22"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="22" t="s">
         <v>54</v>
       </c>
@@ -1415,17 +1464,19 @@
       <c r="E20" s="40" t="s">
         <v>56</v>
       </c>
+      <c r="F20" s="42"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="26" t="n"/>
-      <c r="B21" s="29" t="n"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="28" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="33" t="n"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1436,8 +1487,8 @@
     <mergeCell ref="B12:B13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E4" display="Sch_ool.1a@gmail.com" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E14" display="Sch_ool.1a@gmail.com" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId1" display="Sch_ool.1a@gmail.com" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E14" r:id="rId2" display="Sch_ool.1a@gmail.com" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>